<commit_message>
update v0.21 (replace '-' with '_' in item names)
Item names originally had '-' between words to match the original NIMH EMA names, the '-' were replaced with '_' to accomodate parsing in js
</commit_message>
<xml_diff>
--- a/NIMH_to_ML_content_changelog.xlsx
+++ b/NIMH_to_ML_content_changelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike.xiao/Documents/GitHub/HBN_EMA_NIMH2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2208B00-F6A6-8B42-887B-886918906C14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF12735-A078-F348-8949-62119E806797}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="1140" windowWidth="37160" windowHeight="20800" xr2:uid="{6FEE7D1A-8B9B-6344-8FC9-1E27BFFD5055}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="543">
   <si>
     <t>name_pre_v20</t>
   </si>
@@ -677,45 +677,18 @@
     <t>question was added by CMI group</t>
   </si>
   <si>
-    <t>morning-bedtime</t>
-  </si>
-  <si>
     <t>About what time did you go to bed last night (regardless of the time you actually fell asleep)?</t>
   </si>
   <si>
     <t>new</t>
   </si>
   <si>
-    <t>morning-close-eyes</t>
-  </si>
-  <si>
-    <t>morning-sleep-latency</t>
-  </si>
-  <si>
-    <t>morning-wake-number</t>
-  </si>
-  <si>
-    <t>morning-lights-off</t>
-  </si>
-  <si>
-    <t>morning-waketime</t>
-  </si>
-  <si>
-    <t>morning-outbed</t>
-  </si>
-  <si>
-    <t>morning-sleep-quantity</t>
-  </si>
-  <si>
     <t>morning-sleep-quality</t>
   </si>
   <si>
     <t>socialmedia</t>
   </si>
   <si>
-    <t>socialmedia-type</t>
-  </si>
-  <si>
     <t>About how many hours did you actually sleep?</t>
   </si>
   <si>
@@ -731,18 +704,9 @@
     <t>How rested did you feel upon awakening?</t>
   </si>
   <si>
-    <t>morning-sleep-problems</t>
-  </si>
-  <si>
     <t>Which (if any) of the following sleep problems did you have last night?</t>
   </si>
   <si>
-    <t>morning-sleep-problems-reason</t>
-  </si>
-  <si>
-    <t>morning-sleeping-pills</t>
-  </si>
-  <si>
     <t>Did you take any sleeping pills last night?</t>
   </si>
   <si>
@@ -755,60 +719,24 @@
     <t>In the ML version, 'or anything else to help you sleep last night' was added to the question</t>
   </si>
   <si>
-    <t>socialmedia-after-bedtime</t>
-  </si>
-  <si>
-    <t>socialmedia-fall-asleep</t>
-  </si>
-  <si>
-    <t>since-activity-monitor</t>
-  </si>
-  <si>
-    <t>since-activity-monitor-time</t>
-  </si>
-  <si>
-    <t>now-where</t>
-  </si>
-  <si>
     <t>Where are you right now?</t>
   </si>
   <si>
-    <t>since-where</t>
-  </si>
-  <si>
-    <t>now-company</t>
-  </si>
-  <si>
     <t>Who is with you at this moment?</t>
   </si>
   <si>
     <t>In the ML version, response 'family members or partner' was changed to 'family members', 'partner/boyfriend/girlfriend' was added</t>
   </si>
   <si>
-    <t>since-company</t>
-  </si>
-  <si>
-    <t>now-activity</t>
-  </si>
-  <si>
     <t>What are you doing at this moment?</t>
   </si>
   <si>
     <t>In the ML version, responses 'homework', 'reading', texting by phone' was added</t>
   </si>
   <si>
-    <t>since-activity</t>
-  </si>
-  <si>
-    <t>now-sadness</t>
-  </si>
-  <si>
     <t>How happy versus sad do you feel right now?</t>
   </si>
   <si>
-    <t>now-anxiousness</t>
-  </si>
-  <si>
     <t>How relaxed vs. anxious do you feel right now?</t>
   </si>
   <si>
@@ -818,15 +746,6 @@
     <t>name_NIMH_renamed</t>
   </si>
   <si>
-    <t>morning-sleep-refreshed</t>
-  </si>
-  <si>
-    <t>now-energy</t>
-  </si>
-  <si>
-    <t>now-distracted</t>
-  </si>
-  <si>
     <t>How well can you concentrate or focus right now?</t>
   </si>
   <si>
@@ -839,33 +758,15 @@
     <t>In the ML version, the word 'rested' was changed to 'refreshed' in both the question and responses, 'upon awakening' was changed to 'when you woke up'. The question was renamed from 'morning-sleep-quality' to 'morning-sleep-refreshed'.</t>
   </si>
   <si>
-    <t>now-irritable</t>
-  </si>
-  <si>
     <t>How irritable or easily angered do you feel right now?</t>
   </si>
   <si>
-    <t>now-worried</t>
-  </si>
-  <si>
-    <t>now-guilty</t>
-  </si>
-  <si>
-    <t>now-decisions</t>
-  </si>
-  <si>
     <t>now-slow-thinking</t>
   </si>
   <si>
-    <t>now-quick-thinking</t>
-  </si>
-  <si>
     <t>How quick is your thinking?</t>
   </si>
   <si>
-    <t>now-enjoyment</t>
-  </si>
-  <si>
     <t>How much are you able to enjoy and feel pleasure in things?</t>
   </si>
   <si>
@@ -878,33 +779,9 @@
     <t>How fidgety or restless do you feel right now compared to your usual self?</t>
   </si>
   <si>
-    <t>now-fidgety</t>
-  </si>
-  <si>
-    <t>now-hungry</t>
-  </si>
-  <si>
     <t>How hungry do you feel right now?</t>
   </si>
   <si>
-    <t>now-sleepy</t>
-  </si>
-  <si>
-    <t>now-thoughts-positive</t>
-  </si>
-  <si>
-    <t>now-thoughts-negative</t>
-  </si>
-  <si>
-    <t>now-thoughts-negative-about</t>
-  </si>
-  <si>
-    <t>now-thoughts-negative-severity</t>
-  </si>
-  <si>
-    <t>since-rest</t>
-  </si>
-  <si>
     <t>Since the last assessment, did you have a nap or rest?</t>
   </si>
   <si>
@@ -914,24 +791,15 @@
     <t>practically_identical</t>
   </si>
   <si>
-    <t>since-rest-duration</t>
-  </si>
-  <si>
     <t>How long was your nap or rest?</t>
   </si>
   <si>
     <t>In the ML version, the word 'about' was added to the beginning of the question</t>
   </si>
   <si>
-    <t>since-rest-fell-asleep</t>
-  </si>
-  <si>
     <t>Did you actually fall asleep during the nap or rest?</t>
   </si>
   <si>
-    <t>since-physical-activity</t>
-  </si>
-  <si>
     <t>Which places have you been **since you woke up/since the last questionnaire**?</t>
   </si>
   <si>
@@ -950,9 +818,6 @@
     <t>in the ML version, choices are stored as an array, in the NIMH version, each choice are stored as a new 0,1 variable with the name of the choice appended to the question name</t>
   </si>
   <si>
-    <t>since-vigorous-activity</t>
-  </si>
-  <si>
     <t>Since you woke up/Since the last questionnaire, how many minutes did you do **vigorous activities** including intensive sports or exercise (such as running or fast cycling) or intensive physical work (such as heavy lifting or digging)?</t>
   </si>
   <si>
@@ -965,144 +830,60 @@
     <t>Since you woke up/Since the last questionnaire, how many minutes did you do vigorous activities including intensive sports or exercise (such as running or fast cycling) or intensive physical work (such as heavy lifting or digging)?</t>
   </si>
   <si>
-    <t>since-vigorous-activity-planned</t>
-  </si>
-  <si>
     <t>Was this vigorous activity (or activities) part of a planned workout or exercise routine?</t>
   </si>
   <si>
-    <t>since-moderate-activity</t>
-  </si>
-  <si>
     <t>Since you woke up/Since the last questionnaire, how many minutes did you do moderate activities (activities that make you breathe somewhat harder than usual such as playing tennis, bicycling, carrying light loads)?</t>
   </si>
   <si>
-    <t>since-moderate-activity-planned</t>
-  </si>
-  <si>
     <t>Was this moderate activity (or activities) part of a planned workout or exercise routine?</t>
   </si>
   <si>
-    <t>since-light-activity</t>
-  </si>
-  <si>
     <t>Since you woke up/Since the last questionnaire, how many minutes did you do light activities (activities that may not make you breathe somewhat harder than usual such as walking, climbing stairs, routine household chores, etc.)?</t>
   </si>
   <si>
-    <t>since-light-activity-planned</t>
-  </si>
-  <si>
     <t>Was this light activity (or activities) part of a planned workout or exercise routine?</t>
   </si>
   <si>
-    <t>since-had-drink</t>
-  </si>
-  <si>
     <t>Since you woke up/Since the last questionnaire, did you drink:</t>
   </si>
   <si>
     <t>in the ML version, choices are stored as an array, in the NIMH version, each choice are stored as a new 0,1 variable with the name of the choice appended to the question name, added 'none' option</t>
   </si>
   <si>
-    <t>since-had-drink-water-quantity</t>
-  </si>
-  <si>
     <t>How many 8 oz glasses of water did you consume?</t>
   </si>
   <si>
-    <t>since-had-drink-milk-quantity</t>
-  </si>
-  <si>
     <t>How many 8 oz glasses of milk did you consume?</t>
   </si>
   <si>
-    <t>since-had-drink-caffeinated-type</t>
-  </si>
-  <si>
     <t>What type of caffeinated beverage did you consume?</t>
   </si>
   <si>
-    <t>since-had-drink-caffeinated-quantity</t>
-  </si>
-  <si>
     <t>How many 8 oz glasses of caffeinated drinks did you consume?</t>
   </si>
   <si>
-    <t>since-had-drink-alcohol-type</t>
-  </si>
-  <si>
     <t>What type of alcoholic beverage did you consume?</t>
   </si>
   <si>
-    <t>since-had-drink-alcohol-quantity</t>
-  </si>
-  <si>
     <t>How many servings of alcohol did you consume?</t>
   </si>
   <si>
-    <t>since-had-drink-sugar-quantity</t>
-  </si>
-  <si>
     <t>How many 8 oz glasses of high-sugar drinks (e.g., juice, soda, some coffee beverages) did you consume?</t>
   </si>
   <si>
-    <t>since-eaten-type</t>
-  </si>
-  <si>
     <t>question was added by NIMH group, food section was revamped</t>
   </si>
   <si>
-    <t>since-eaten-snacks-quantity</t>
-  </si>
-  <si>
     <t>Since you woke up/Since the last questionnaire, which of the following did you have?</t>
   </si>
   <si>
-    <t>since-eaten-small-meal-quantity</t>
-  </si>
-  <si>
-    <t>since-eaten-regular-meal-quantity</t>
-  </si>
-  <si>
-    <t>since-eaten-large-meal-quantity</t>
-  </si>
-  <si>
-    <t>since-eaten-amount</t>
-  </si>
-  <si>
     <t>About **what time** did you eat your largest snack/meal?</t>
   </si>
   <si>
-    <t>since-eaten-when</t>
-  </si>
-  <si>
-    <t>since-eaten-duration</t>
-  </si>
-  <si>
-    <t>since-eaten-chocolate</t>
-  </si>
-  <si>
-    <t>since-substances</t>
-  </si>
-  <si>
     <t>Since you woke up/since the last questionnaire, which of the following did you use?</t>
   </si>
   <si>
-    <t>since-substances-cigarettes</t>
-  </si>
-  <si>
-    <t>since-substances-cannabis</t>
-  </si>
-  <si>
-    <t>since-substances-other</t>
-  </si>
-  <si>
-    <t>event-instructions</t>
-  </si>
-  <si>
-    <t>event-category</t>
-  </si>
-  <si>
     <t>Which of the following categories best describes the area of your life in which the event occurred?</t>
   </si>
   <si>
@@ -1133,45 +914,15 @@
     <t>in the ML version, choices are stored as an array, in the NIMH version, each choice are stored as a new 0,1 variable with the name of the choice appended to the question name, removed 'painkiller' choice, changed 'heroin' to 'heroin or other opiate', added the word 'other' in question</t>
   </si>
   <si>
-    <t>event-impact-positive</t>
-  </si>
-  <si>
-    <t>event-impact-negative</t>
-  </si>
-  <si>
     <t>In NIMH version, there is a question that asked 'To what degree did this event have a positive or negative impact on you?' This was split into two new questions 'event-impact-positive' and 'event-impact-negative' in the ML version</t>
   </si>
   <si>
-    <t>event-other</t>
-  </si>
-  <si>
-    <t>event-other-impact-positive</t>
-  </si>
-  <si>
-    <t>event-other-impact-negative</t>
-  </si>
-  <si>
     <t>now-pain</t>
   </si>
   <si>
-    <t>now-pain-where</t>
-  </si>
-  <si>
     <t>In the NIMH version, there was a question named 'now-pain' that read 'Are you in pain right now (other than headache pain)?'. The responses to this question were in the form of a 1-7 likert scale, with 1 = 'no pain', 7 = 'extreme pain'. May be similar enough to merge with the ML version question in some cases</t>
   </si>
   <si>
-    <t>now-pain-level</t>
-  </si>
-  <si>
-    <t>since-pain</t>
-  </si>
-  <si>
-    <t>since-pain-where</t>
-  </si>
-  <si>
-    <t>since-pain-level</t>
-  </si>
-  <si>
     <t>Are you in pain right now (other than headache pain)?</t>
   </si>
   <si>
@@ -1196,12 +947,6 @@
     <t>since-headache/now-headache</t>
   </si>
   <si>
-    <t>headache-same</t>
-  </si>
-  <si>
-    <t>headache-prevent</t>
-  </si>
-  <si>
     <t>prevention-actions</t>
   </si>
   <si>
@@ -1220,21 +965,12 @@
     <t>In the NIMH version, this question was given conditionally on the user saying 'no' to having a headache since the last questionnaire. In the ML version, the question is given unconditionally. In the morning assessments, this question will no longer say 'since you woke up' in order to be consistent with the wording of 'headache'. The question was renamed from 'prevention-action' to 'headache-prevent'.</t>
   </si>
   <si>
-    <t>headache-start</t>
-  </si>
-  <si>
     <t>What time did the headache begin?</t>
   </si>
   <si>
     <t>In the ML version, this question is conditionally  given on 'headache-same' = 'no' to avoid redundancy. In the NIMH version, responses are given in 60 minute intervals via single select, in the ML version, responses are given at the minute level via clock widget</t>
   </si>
   <si>
-    <t>headache-current</t>
-  </si>
-  <si>
-    <t>headache-end</t>
-  </si>
-  <si>
     <t>What time did the headache end?</t>
   </si>
   <si>
@@ -1244,99 +980,48 @@
     <t>The NIMH version of 'headache-end' had  'Headache is still present' as the first choice. In ML, this first option was removed and turned into a new yes/no question 'headache-current'. In the NIMH version, responses are given in 60 minute intervals via single select, in the ML version, responses are given at the minute level via clock widget</t>
   </si>
   <si>
-    <t>headache-intensity</t>
-  </si>
-  <si>
     <t>How intense is (or was) the headache?</t>
   </si>
   <si>
     <t>In the ML version, text for choice 4 'moderately intense' was removed, leaving just 'very minor' and 'extremely intense' on choice 1 and 7</t>
   </si>
   <si>
-    <t>headache-sudden</t>
-  </si>
-  <si>
-    <t>headache-trigger</t>
-  </si>
-  <si>
-    <t>headache-trigger-category</t>
-  </si>
-  <si>
-    <t>headache-location</t>
-  </si>
-  <si>
     <t>Where is (or was) the headache?</t>
   </si>
   <si>
-    <t>headache-pulsating</t>
-  </si>
-  <si>
     <t>Is (or was) the pain throbbing, beating or pulsating?</t>
   </si>
   <si>
-    <t>headache-effort</t>
-  </si>
-  <si>
     <t>Does (or did) the headache pain increase with routine physical activity such as bending over or climbing stairs?</t>
   </si>
   <si>
-    <t>headache-nausea</t>
-  </si>
-  <si>
     <t>Do (or did) you feel nauseated, vomit or have diarrhea?</t>
   </si>
   <si>
     <t>In the NIMH version, the responses may actually (erroneously) be a 1-4 scale from 'Not at all' to 'Severely'. Either way, the ML version has yes/no response for this question</t>
   </si>
   <si>
-    <t>headache-light</t>
-  </si>
-  <si>
     <t>How much does (or did) light bother you?</t>
   </si>
   <si>
-    <t>headache-noise</t>
-  </si>
-  <si>
     <t>How much does (or did) noise such as music, talking, TV, bother you?</t>
   </si>
   <si>
-    <t>headache-smell</t>
-  </si>
-  <si>
     <t>question was added by NIMH group, because this question was added, 'headache-odor-trigger' was removed from the ML version</t>
   </si>
   <si>
     <t>How much does (or did) certain odors such as perfume, food, smoke, bother you?</t>
   </si>
   <si>
-    <t>headache-vision-changes</t>
-  </si>
-  <si>
     <t>Which (if any) of the following vision changes did you experience?</t>
   </si>
   <si>
-    <t>headache-vision-change-time</t>
-  </si>
-  <si>
     <t>When did those vision changes occur with respect to the onset of the headache pain?</t>
   </si>
   <si>
-    <t>headache-numbing</t>
-  </si>
-  <si>
     <t>Is (or was) your headache accompanied by any numbing or tingling in certain body areas?</t>
   </si>
   <si>
-    <t>headache-numbing-time</t>
-  </si>
-  <si>
-    <t>headache-confusing</t>
-  </si>
-  <si>
-    <t>headache-confusing-time</t>
-  </si>
-  <si>
     <t>When did this numbing or tingling occur with respect to onset of the headache pain?</t>
   </si>
   <si>
@@ -1349,15 +1034,9 @@
     <t>Did the headache come on suddenly?</t>
   </si>
   <si>
-    <t>headache-medication</t>
-  </si>
-  <si>
     <t>Which (if any) did you take to treat your headache?</t>
   </si>
   <si>
-    <t>headache-interference</t>
-  </si>
-  <si>
     <t>How much does (or did) the headache interfere with your activities?</t>
   </si>
   <si>
@@ -1523,81 +1202,24 @@
     <t>**How many hours** did you spend on **social media** today?</t>
   </si>
   <si>
-    <t>day-stress</t>
-  </si>
-  <si>
-    <t>day-stress-category</t>
-  </si>
-  <si>
     <t>question was added by NIMH group. question from NIMH palm version (older) could potentially be merged with this one</t>
   </si>
   <si>
-    <t>day-stress-typical</t>
-  </si>
-  <si>
-    <t>day-routine-typical</t>
-  </si>
-  <si>
-    <t>day-phyiscal-health</t>
-  </si>
-  <si>
     <t>How was your physical health today?</t>
   </si>
   <si>
-    <t>day-over-medication</t>
-  </si>
-  <si>
     <t>Did you take any over-the-counter medications today?</t>
   </si>
   <si>
-    <t>day-over-medication-why</t>
-  </si>
-  <si>
-    <t>day-prescribed-medication</t>
-  </si>
-  <si>
     <t>Did you take any prescription medications today?</t>
   </si>
   <si>
-    <t>day-prescribed-medication-conditions</t>
-  </si>
-  <si>
-    <t>day-period</t>
-  </si>
-  <si>
     <t>Are you currently having your period?</t>
   </si>
   <si>
-    <t>day-lethargic</t>
-  </si>
-  <si>
     <t>Did you feel like you had no physical energy, as if you were weighted down or had a heavy feeling in your arms and legs for most of the day?</t>
   </si>
   <si>
-    <t>day-cold-cough-flu</t>
-  </si>
-  <si>
-    <t>day-problem-categories</t>
-  </si>
-  <si>
-    <t>day-problems-allergies</t>
-  </si>
-  <si>
-    <t>day-problems-breath</t>
-  </si>
-  <si>
-    <t>day-problems-belly-symptoms</t>
-  </si>
-  <si>
-    <t>day-problems-belly</t>
-  </si>
-  <si>
-    <t>day-problems-muscle</t>
-  </si>
-  <si>
-    <t>day-problems-heart</t>
-  </si>
-  <si>
     <t>Do you have a cold, cough, or flu today?</t>
   </si>
   <si>
@@ -1625,34 +1247,421 @@
     <t>Did you actually faint today?</t>
   </si>
   <si>
-    <t>diziness-situation</t>
-  </si>
-  <si>
-    <t>diziness-faint</t>
-  </si>
-  <si>
-    <t>day-headache-duration</t>
-  </si>
-  <si>
-    <t>internet-use-duration</t>
-  </si>
-  <si>
-    <t>internet-use-category</t>
-  </si>
-  <si>
-    <t>internet-use-location</t>
-  </si>
-  <si>
-    <t>socialmedia-duration</t>
-  </si>
-  <si>
-    <t>friends-communication-method</t>
-  </si>
-  <si>
     <t>Did these feelings occur in a particular situation (in a bus, in hot weather, or other condition)?</t>
   </si>
   <si>
     <t>In the ML version, the phrase 'of dizziness' was added and 'diziness-instructions' removed</t>
+  </si>
+  <si>
+    <t>socialmedia_type</t>
+  </si>
+  <si>
+    <t>morning_bedtime</t>
+  </si>
+  <si>
+    <t>morning_lights_off</t>
+  </si>
+  <si>
+    <t>morning_close_eyes</t>
+  </si>
+  <si>
+    <t>morning_sleep_latency</t>
+  </si>
+  <si>
+    <t>morning_wake_number</t>
+  </si>
+  <si>
+    <t>morning_waketime</t>
+  </si>
+  <si>
+    <t>morning_outbed</t>
+  </si>
+  <si>
+    <t>morning_sleep_quantity</t>
+  </si>
+  <si>
+    <t>morning_sleep_quality</t>
+  </si>
+  <si>
+    <t>morning_sleep_refreshed</t>
+  </si>
+  <si>
+    <t>morning_sleep_problems</t>
+  </si>
+  <si>
+    <t>morning_sleep_problems_reason</t>
+  </si>
+  <si>
+    <t>morning_sleeping_pills</t>
+  </si>
+  <si>
+    <t>socialmedia_after_bedtime</t>
+  </si>
+  <si>
+    <t>socialmedia_fall_asleep</t>
+  </si>
+  <si>
+    <t>since_activity_monitor</t>
+  </si>
+  <si>
+    <t>since_activity_monitor_time</t>
+  </si>
+  <si>
+    <t>now_where</t>
+  </si>
+  <si>
+    <t>since_where</t>
+  </si>
+  <si>
+    <t>now_company</t>
+  </si>
+  <si>
+    <t>since_company</t>
+  </si>
+  <si>
+    <t>now_activity</t>
+  </si>
+  <si>
+    <t>since_activity</t>
+  </si>
+  <si>
+    <t>now_sadness</t>
+  </si>
+  <si>
+    <t>now_anxiousness</t>
+  </si>
+  <si>
+    <t>now_excited</t>
+  </si>
+  <si>
+    <t>now_energy</t>
+  </si>
+  <si>
+    <t>now_distracted</t>
+  </si>
+  <si>
+    <t>now_irritable</t>
+  </si>
+  <si>
+    <t>now_worried</t>
+  </si>
+  <si>
+    <t>now_guilty</t>
+  </si>
+  <si>
+    <t>now_decisions</t>
+  </si>
+  <si>
+    <t>now_quick_thinking</t>
+  </si>
+  <si>
+    <t>now_enjoyment</t>
+  </si>
+  <si>
+    <t>now_fidgety</t>
+  </si>
+  <si>
+    <t>now_hungry</t>
+  </si>
+  <si>
+    <t>now_sleepy</t>
+  </si>
+  <si>
+    <t>now_thoughts_positive</t>
+  </si>
+  <si>
+    <t>now_thoughts_negative</t>
+  </si>
+  <si>
+    <t>now_thoughts_negative_about</t>
+  </si>
+  <si>
+    <t>now_thoughts_negative_severity</t>
+  </si>
+  <si>
+    <t>since_rest</t>
+  </si>
+  <si>
+    <t>since_rest_duration</t>
+  </si>
+  <si>
+    <t>since_rest_fell_asleep</t>
+  </si>
+  <si>
+    <t>since_physical_activity</t>
+  </si>
+  <si>
+    <t>since_vigorous_activity</t>
+  </si>
+  <si>
+    <t>since_vigorous_activity_planned</t>
+  </si>
+  <si>
+    <t>since_moderate_activity</t>
+  </si>
+  <si>
+    <t>since_moderate_activity_planned</t>
+  </si>
+  <si>
+    <t>since_light_activity</t>
+  </si>
+  <si>
+    <t>since_light_activity_planned</t>
+  </si>
+  <si>
+    <t>since_had_drink</t>
+  </si>
+  <si>
+    <t>since_had_drink_water_quantity</t>
+  </si>
+  <si>
+    <t>since_had_drink_milk_quantity</t>
+  </si>
+  <si>
+    <t>since_had_drink_caffeinated_type</t>
+  </si>
+  <si>
+    <t>since_had_drink_caffeinated_quantity</t>
+  </si>
+  <si>
+    <t>since_had_drink_alcohol_type</t>
+  </si>
+  <si>
+    <t>since_had_drink_alcohol_quantity</t>
+  </si>
+  <si>
+    <t>since_had_drink_sugar_quantity</t>
+  </si>
+  <si>
+    <t>since_eaten_amount</t>
+  </si>
+  <si>
+    <t>since_eaten_snacks_quantity</t>
+  </si>
+  <si>
+    <t>since_eaten_small_meal_quantity</t>
+  </si>
+  <si>
+    <t>since_eaten_regular_meal_quantity</t>
+  </si>
+  <si>
+    <t>since_eaten_large_meal_quantity</t>
+  </si>
+  <si>
+    <t>since_eaten_when</t>
+  </si>
+  <si>
+    <t>since_eaten_duration</t>
+  </si>
+  <si>
+    <t>since_eaten_type</t>
+  </si>
+  <si>
+    <t>since_eaten_chocolate</t>
+  </si>
+  <si>
+    <t>since_substances</t>
+  </si>
+  <si>
+    <t>since_substances_cigarettes</t>
+  </si>
+  <si>
+    <t>since_substances_cannabis</t>
+  </si>
+  <si>
+    <t>since_substances_other</t>
+  </si>
+  <si>
+    <t>event_instructions</t>
+  </si>
+  <si>
+    <t>event_category</t>
+  </si>
+  <si>
+    <t>event_impact_positive</t>
+  </si>
+  <si>
+    <t>event_impact_negative</t>
+  </si>
+  <si>
+    <t>event_other</t>
+  </si>
+  <si>
+    <t>event_other_impact_positive</t>
+  </si>
+  <si>
+    <t>event_other_impact_negative</t>
+  </si>
+  <si>
+    <t>now_pain</t>
+  </si>
+  <si>
+    <t>now_pain_where</t>
+  </si>
+  <si>
+    <t>now_pain_level</t>
+  </si>
+  <si>
+    <t>since_pain</t>
+  </si>
+  <si>
+    <t>since_pain_where</t>
+  </si>
+  <si>
+    <t>since_pain_level</t>
+  </si>
+  <si>
+    <t>headache_same</t>
+  </si>
+  <si>
+    <t>headache_prevent</t>
+  </si>
+  <si>
+    <t>headache_start</t>
+  </si>
+  <si>
+    <t>headache_current</t>
+  </si>
+  <si>
+    <t>headache_end</t>
+  </si>
+  <si>
+    <t>headache_intensity</t>
+  </si>
+  <si>
+    <t>headache_sudden</t>
+  </si>
+  <si>
+    <t>headache_trigger</t>
+  </si>
+  <si>
+    <t>headache_trigger_category</t>
+  </si>
+  <si>
+    <t>headache_location</t>
+  </si>
+  <si>
+    <t>headache_pulsating</t>
+  </si>
+  <si>
+    <t>headache_effort</t>
+  </si>
+  <si>
+    <t>headache_nausea</t>
+  </si>
+  <si>
+    <t>headache_light</t>
+  </si>
+  <si>
+    <t>headache_noise</t>
+  </si>
+  <si>
+    <t>headache_smell</t>
+  </si>
+  <si>
+    <t>headache_vision_changes</t>
+  </si>
+  <si>
+    <t>headache_vision_change_time</t>
+  </si>
+  <si>
+    <t>headache_numbing</t>
+  </si>
+  <si>
+    <t>headache_numbing_time</t>
+  </si>
+  <si>
+    <t>headache_confusing</t>
+  </si>
+  <si>
+    <t>headache_confusing_time</t>
+  </si>
+  <si>
+    <t>headache_medication</t>
+  </si>
+  <si>
+    <t>headache_interference</t>
+  </si>
+  <si>
+    <t>day_stress</t>
+  </si>
+  <si>
+    <t>day_stress_category</t>
+  </si>
+  <si>
+    <t>day_stress_typical</t>
+  </si>
+  <si>
+    <t>day_routine_typical</t>
+  </si>
+  <si>
+    <t>day_phyiscal_health</t>
+  </si>
+  <si>
+    <t>day_over_medication</t>
+  </si>
+  <si>
+    <t>day_over_medication_why</t>
+  </si>
+  <si>
+    <t>day_prescribed_medication</t>
+  </si>
+  <si>
+    <t>day_prescribed_medication_conditions</t>
+  </si>
+  <si>
+    <t>day_period</t>
+  </si>
+  <si>
+    <t>day_lethargic</t>
+  </si>
+  <si>
+    <t>day_cold_cough_flu</t>
+  </si>
+  <si>
+    <t>day_problem_categories</t>
+  </si>
+  <si>
+    <t>day_problems_allergies</t>
+  </si>
+  <si>
+    <t>day_problems_breath</t>
+  </si>
+  <si>
+    <t>day_problems_belly_symptoms</t>
+  </si>
+  <si>
+    <t>day_problems_belly</t>
+  </si>
+  <si>
+    <t>day_problems_muscle</t>
+  </si>
+  <si>
+    <t>day_problems_heart</t>
+  </si>
+  <si>
+    <t>diziness_situation</t>
+  </si>
+  <si>
+    <t>diziness_faint</t>
+  </si>
+  <si>
+    <t>day_headache_duration</t>
+  </si>
+  <si>
+    <t>internet_use_duration</t>
+  </si>
+  <si>
+    <t>internet_use_category</t>
+  </si>
+  <si>
+    <t>internet_use_location</t>
+  </si>
+  <si>
+    <t>friends_communication_method</t>
+  </si>
+  <si>
+    <t>socialmedia_duration</t>
   </si>
 </sst>
 </file>
@@ -2011,7 +2020,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C146" sqref="C146"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2032,10 +2041,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C1" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -2044,10 +2053,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G1" t="s">
-        <v>292</v>
+        <v>251</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -2061,7 +2070,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>117</v>
@@ -2078,7 +2087,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>406</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>118</v>
@@ -2095,13 +2104,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>407</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>119</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -2113,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2121,7 +2130,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>408</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>120</v>
@@ -2130,7 +2139,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2138,7 +2147,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>409</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>121</v>
@@ -2147,7 +2156,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2155,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>218</v>
+        <v>410</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>122</v>
@@ -2164,7 +2173,7 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2172,7 +2181,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>219</v>
+        <v>411</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>123</v>
@@ -2181,7 +2190,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2189,7 +2198,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>412</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>124</v>
@@ -2198,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2206,7 +2215,7 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>413</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>125</v>
@@ -2215,7 +2224,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2223,13 +2232,13 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>223</v>
+        <v>414</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -2241,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2249,7 +2258,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>224</v>
+        <v>415</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>127</v>
@@ -2258,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -2266,16 +2275,16 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>261</v>
+        <v>416</v>
       </c>
       <c r="C13" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>128</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -2287,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>267</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2295,13 +2304,13 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>232</v>
+        <v>417</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>129</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -2313,7 +2322,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2321,7 +2330,7 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>234</v>
+        <v>418</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>130</v>
@@ -2330,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2338,13 +2347,13 @@
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>235</v>
+        <v>419</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>131</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -2356,7 +2365,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2364,7 +2373,7 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>240</v>
+        <v>420</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>132</v>
@@ -2381,7 +2390,7 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>241</v>
+        <v>421</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>133</v>
@@ -2398,7 +2407,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>242</v>
+        <v>422</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>134</v>
@@ -2407,7 +2416,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2415,7 +2424,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>243</v>
+        <v>423</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>135</v>
@@ -2424,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2432,13 +2441,13 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>244</v>
+        <v>424</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>136</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -2450,7 +2459,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2458,16 +2467,16 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>246</v>
+        <v>425</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>299</v>
+        <v>255</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2475,13 +2484,13 @@
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>247</v>
+        <v>426</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>137</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -2493,7 +2502,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2501,16 +2510,16 @@
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>250</v>
+        <v>427</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="F24" s="1">
         <v>1</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2518,13 +2527,13 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>251</v>
+        <v>428</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -2536,7 +2545,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2544,16 +2553,16 @@
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>254</v>
+        <v>429</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>301</v>
+        <v>257</v>
       </c>
       <c r="F26" s="1">
         <v>1</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2561,13 +2570,13 @@
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>255</v>
+        <v>430</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>139</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -2584,13 +2593,13 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>257</v>
+        <v>431</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>140</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -2607,7 +2616,7 @@
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>259</v>
+        <v>432</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>141</v>
@@ -2616,7 +2625,7 @@
         <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2624,16 +2633,16 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>262</v>
+        <v>433</v>
       </c>
       <c r="C30" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>142</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2645,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2653,13 +2662,13 @@
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>263</v>
+        <v>434</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2676,13 +2685,13 @@
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>268</v>
+        <v>435</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>144</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2699,7 +2708,7 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>270</v>
+        <v>436</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>145</v>
@@ -2708,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2716,7 +2725,7 @@
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>271</v>
+        <v>437</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>146</v>
@@ -2725,7 +2734,7 @@
         <v>1</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2733,7 +2742,7 @@
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>272</v>
+        <v>438</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>147</v>
@@ -2742,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2750,16 +2759,16 @@
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>274</v>
+        <v>439</v>
       </c>
       <c r="C36" t="s">
-        <v>273</v>
+        <v>242</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
@@ -2771,7 +2780,7 @@
         <v>1</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2779,13 +2788,13 @@
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>276</v>
+        <v>440</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>149</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>277</v>
+        <v>244</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -2797,7 +2806,7 @@
         <v>1</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>279</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2805,13 +2814,13 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>281</v>
+        <v>441</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>150</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>280</v>
+        <v>247</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -2828,13 +2837,13 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>282</v>
+        <v>442</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>283</v>
+        <v>248</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
@@ -2851,7 +2860,7 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>284</v>
+        <v>443</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>152</v>
@@ -2860,7 +2869,7 @@
         <v>1</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2868,7 +2877,7 @@
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>285</v>
+        <v>444</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>153</v>
@@ -2877,7 +2886,7 @@
         <v>1</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -2885,7 +2894,7 @@
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>286</v>
+        <v>445</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>154</v>
@@ -2894,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2902,7 +2911,7 @@
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>287</v>
+        <v>446</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>155</v>
@@ -2911,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2919,7 +2928,7 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>288</v>
+        <v>447</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>156</v>
@@ -2928,7 +2937,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2936,13 +2945,13 @@
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>289</v>
+        <v>448</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>157</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
@@ -2954,7 +2963,7 @@
         <v>1</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>291</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2962,13 +2971,13 @@
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>293</v>
+        <v>449</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>158</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>294</v>
+        <v>252</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -2980,7 +2989,7 @@
         <v>1</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>295</v>
+        <v>253</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -2988,13 +2997,13 @@
         <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>296</v>
+        <v>450</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>159</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
@@ -3011,13 +3020,13 @@
         <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>298</v>
+        <v>451</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>303</v>
+        <v>259</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>302</v>
+        <v>258</v>
       </c>
       <c r="F48" s="1">
         <v>0</v>
@@ -3029,7 +3038,7 @@
         <v>1</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -3037,13 +3046,13 @@
         <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>305</v>
+        <v>452</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>306</v>
+        <v>261</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>309</v>
+        <v>264</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
@@ -3060,13 +3069,13 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>310</v>
+        <v>453</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>311</v>
+        <v>265</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
@@ -3083,13 +3092,13 @@
         <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>312</v>
+        <v>454</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>307</v>
+        <v>262</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>313</v>
+        <v>266</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
@@ -3106,13 +3115,13 @@
         <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>314</v>
+        <v>455</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>161</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>315</v>
+        <v>267</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
@@ -3129,13 +3138,13 @@
         <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>316</v>
+        <v>456</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>308</v>
+        <v>263</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>317</v>
+        <v>268</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
@@ -3152,13 +3161,13 @@
         <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>318</v>
+        <v>457</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>162</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>319</v>
+        <v>269</v>
       </c>
       <c r="F54" s="1">
         <v>0</v>
@@ -3175,13 +3184,13 @@
         <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>320</v>
+        <v>458</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>321</v>
+        <v>270</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
@@ -3193,7 +3202,7 @@
         <v>1</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3201,13 +3210,13 @@
         <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>323</v>
+        <v>459</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>324</v>
+        <v>272</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -3224,13 +3233,13 @@
         <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>325</v>
+        <v>460</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>164</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>326</v>
+        <v>273</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -3247,13 +3256,13 @@
         <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>327</v>
+        <v>461</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>165</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>328</v>
+        <v>274</v>
       </c>
       <c r="F58" s="1">
         <v>0</v>
@@ -3265,7 +3274,7 @@
         <v>1</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3273,13 +3282,13 @@
         <v>62</v>
       </c>
       <c r="B59" t="s">
-        <v>329</v>
+        <v>462</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>166</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>330</v>
+        <v>275</v>
       </c>
       <c r="F59" s="1">
         <v>0</v>
@@ -3296,13 +3305,13 @@
         <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>331</v>
+        <v>463</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>167</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>332</v>
+        <v>276</v>
       </c>
       <c r="F60" s="1">
         <v>0</v>
@@ -3314,7 +3323,7 @@
         <v>1</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3322,13 +3331,13 @@
         <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>333</v>
+        <v>464</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>168</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>334</v>
+        <v>277</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -3345,13 +3354,13 @@
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>335</v>
+        <v>465</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>169</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>336</v>
+        <v>278</v>
       </c>
       <c r="F62" s="1">
         <v>0</v>
@@ -3368,16 +3377,16 @@
         <v>66</v>
       </c>
       <c r="B63" t="s">
-        <v>344</v>
+        <v>466</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>340</v>
+        <v>280</v>
       </c>
       <c r="F63" s="1">
         <v>1</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>338</v>
+        <v>279</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3385,7 +3394,7 @@
         <v>67</v>
       </c>
       <c r="B64" t="s">
-        <v>339</v>
+        <v>467</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>170</v>
@@ -3394,7 +3403,7 @@
         <v>1</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>338</v>
+        <v>279</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3402,7 +3411,7 @@
         <v>68</v>
       </c>
       <c r="B65" t="s">
-        <v>341</v>
+        <v>468</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>171</v>
@@ -3411,7 +3420,7 @@
         <v>1</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>338</v>
+        <v>279</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3419,7 +3428,7 @@
         <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>342</v>
+        <v>469</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>172</v>
@@ -3428,7 +3437,7 @@
         <v>1</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>338</v>
+        <v>279</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3436,7 +3445,7 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>343</v>
+        <v>470</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>173</v>
@@ -3445,7 +3454,7 @@
         <v>1</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>338</v>
+        <v>279</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3453,13 +3462,13 @@
         <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>346</v>
+        <v>471</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>345</v>
+        <v>281</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>357</v>
+        <v>284</v>
       </c>
       <c r="F68" s="1">
         <v>0</v>
@@ -3471,7 +3480,7 @@
         <v>1</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3479,7 +3488,7 @@
         <v>72</v>
       </c>
       <c r="B69" t="s">
-        <v>347</v>
+        <v>472</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>174</v>
@@ -3488,7 +3497,7 @@
         <v>1</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3496,13 +3505,13 @@
         <v>73</v>
       </c>
       <c r="B70" t="s">
-        <v>337</v>
+        <v>473</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>358</v>
+        <v>285</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>359</v>
+        <v>286</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
@@ -3519,7 +3528,7 @@
         <v>74</v>
       </c>
       <c r="B71" t="s">
-        <v>348</v>
+        <v>474</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>175</v>
@@ -3542,13 +3551,13 @@
         <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>349</v>
+        <v>475</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>350</v>
+        <v>282</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>360</v>
+        <v>287</v>
       </c>
       <c r="F72" s="1">
         <v>0</v>
@@ -3560,7 +3569,7 @@
         <v>1</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>361</v>
+        <v>288</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3568,13 +3577,13 @@
         <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>351</v>
+        <v>476</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>176</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>362</v>
+        <v>289</v>
       </c>
       <c r="F73" s="1">
         <v>0</v>
@@ -3591,13 +3600,13 @@
         <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>352</v>
+        <v>477</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>177</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>363</v>
+        <v>290</v>
       </c>
       <c r="F74" s="1">
         <v>0</v>
@@ -3614,13 +3623,13 @@
         <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>353</v>
+        <v>478</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>178</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>364</v>
+        <v>291</v>
       </c>
       <c r="F75" s="1">
         <v>0</v>
@@ -3632,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>365</v>
+        <v>292</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3640,7 +3649,7 @@
         <v>79</v>
       </c>
       <c r="B76" t="s">
-        <v>354</v>
+        <v>479</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>179</v>
@@ -3660,13 +3669,13 @@
         <v>80</v>
       </c>
       <c r="B77" t="s">
-        <v>355</v>
+        <v>480</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>180</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>356</v>
+        <v>283</v>
       </c>
       <c r="F77" s="1">
         <v>0</v>
@@ -3678,7 +3687,7 @@
         <v>1</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -3686,7 +3695,7 @@
         <v>81</v>
       </c>
       <c r="B78" t="s">
-        <v>366</v>
+        <v>481</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>181</v>
@@ -3695,7 +3704,7 @@
         <v>1</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>368</v>
+        <v>293</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -3703,7 +3712,7 @@
         <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>367</v>
+        <v>482</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>182</v>
@@ -3712,7 +3721,7 @@
         <v>1</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>368</v>
+        <v>293</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3720,7 +3729,7 @@
         <v>83</v>
       </c>
       <c r="B80" t="s">
-        <v>369</v>
+        <v>483</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>183</v>
@@ -3729,7 +3738,7 @@
         <v>1</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3737,7 +3746,7 @@
         <v>84</v>
       </c>
       <c r="B81" t="s">
-        <v>370</v>
+        <v>484</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>184</v>
@@ -3746,7 +3755,7 @@
         <v>1</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3754,7 +3763,7 @@
         <v>85</v>
       </c>
       <c r="B82" t="s">
-        <v>371</v>
+        <v>485</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>185</v>
@@ -3763,7 +3772,7 @@
         <v>1</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3771,7 +3780,7 @@
         <v>86</v>
       </c>
       <c r="B83" t="s">
-        <v>372</v>
+        <v>486</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>186</v>
@@ -3780,7 +3789,7 @@
         <v>1</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3788,7 +3797,7 @@
         <v>87</v>
       </c>
       <c r="B84" t="s">
-        <v>373</v>
+        <v>487</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>187</v>
@@ -3797,7 +3806,7 @@
         <v>1</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -3805,16 +3814,16 @@
         <v>88</v>
       </c>
       <c r="B85" t="s">
-        <v>375</v>
+        <v>488</v>
       </c>
       <c r="C85" t="s">
-        <v>372</v>
+        <v>294</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>188</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>379</v>
+        <v>296</v>
       </c>
       <c r="F85" s="1">
         <v>0</v>
@@ -3826,7 +3835,7 @@
         <v>1</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>374</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3834,13 +3843,13 @@
         <v>89</v>
       </c>
       <c r="B86" t="s">
-        <v>376</v>
+        <v>489</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>380</v>
+        <v>297</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>381</v>
+        <v>298</v>
       </c>
       <c r="F86" s="1">
         <v>0</v>
@@ -3852,7 +3861,7 @@
         <v>1</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>382</v>
+        <v>299</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -3860,7 +3869,7 @@
         <v>90</v>
       </c>
       <c r="B87" t="s">
-        <v>377</v>
+        <v>490</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>189</v>
@@ -3874,13 +3883,13 @@
         <v>91</v>
       </c>
       <c r="B88" t="s">
-        <v>378</v>
+        <v>491</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>383</v>
+        <v>300</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>383</v>
+        <v>300</v>
       </c>
       <c r="F88" s="1">
         <v>0</v>
@@ -3897,16 +3906,16 @@
         <v>92</v>
       </c>
       <c r="B89" t="s">
-        <v>385</v>
+        <v>302</v>
       </c>
       <c r="C89" t="s">
-        <v>386</v>
+        <v>303</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>384</v>
+        <v>301</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>392</v>
+        <v>307</v>
       </c>
       <c r="F89" s="1">
         <v>0</v>
@@ -3918,7 +3927,7 @@
         <v>1</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>393</v>
+        <v>308</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -3926,7 +3935,7 @@
         <v>93</v>
       </c>
       <c r="B90" t="s">
-        <v>387</v>
+        <v>492</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>190</v>
@@ -3935,7 +3944,7 @@
         <v>1</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="102" x14ac:dyDescent="0.2">
@@ -3943,16 +3952,16 @@
         <v>94</v>
       </c>
       <c r="B91" t="s">
-        <v>388</v>
+        <v>493</v>
       </c>
       <c r="C91" t="s">
-        <v>389</v>
+        <v>304</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>390</v>
+        <v>305</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>391</v>
+        <v>306</v>
       </c>
       <c r="F91" s="1">
         <v>0</v>
@@ -3964,7 +3973,7 @@
         <v>1</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>394</v>
+        <v>309</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -3972,13 +3981,13 @@
         <v>95</v>
       </c>
       <c r="B92" t="s">
-        <v>395</v>
+        <v>494</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>191</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>396</v>
+        <v>310</v>
       </c>
       <c r="F92" s="1">
         <v>0</v>
@@ -3990,7 +3999,7 @@
         <v>1</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>397</v>
+        <v>311</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="51" x14ac:dyDescent="0.2">
@@ -3998,7 +4007,7 @@
         <v>96</v>
       </c>
       <c r="B93" t="s">
-        <v>398</v>
+        <v>495</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>192</v>
@@ -4007,7 +4016,7 @@
         <v>1</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>401</v>
+        <v>313</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -4015,13 +4024,13 @@
         <v>97</v>
       </c>
       <c r="B94" t="s">
-        <v>399</v>
+        <v>496</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>193</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>400</v>
+        <v>312</v>
       </c>
       <c r="F94" s="1">
         <v>0</v>
@@ -4033,7 +4042,7 @@
         <v>1</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>402</v>
+        <v>314</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4041,13 +4050,13 @@
         <v>98</v>
       </c>
       <c r="B95" t="s">
-        <v>403</v>
+        <v>497</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>194</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>404</v>
+        <v>315</v>
       </c>
       <c r="F95" s="1">
         <v>0</v>
@@ -4059,7 +4068,7 @@
         <v>1</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>405</v>
+        <v>316</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4067,13 +4076,13 @@
         <v>99</v>
       </c>
       <c r="B96" t="s">
-        <v>406</v>
+        <v>498</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>195</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>437</v>
+        <v>332</v>
       </c>
       <c r="F96" s="1">
         <v>0</v>
@@ -4090,7 +4099,7 @@
         <v>100</v>
       </c>
       <c r="B97" t="s">
-        <v>407</v>
+        <v>499</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>196</v>
@@ -4099,7 +4108,7 @@
         <v>1</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>423</v>
+        <v>324</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4107,7 +4116,7 @@
         <v>101</v>
       </c>
       <c r="B98" t="s">
-        <v>408</v>
+        <v>500</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>197</v>
@@ -4116,7 +4125,7 @@
         <v>1</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>423</v>
+        <v>324</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4124,13 +4133,13 @@
         <v>102</v>
       </c>
       <c r="B99" t="s">
-        <v>409</v>
+        <v>501</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>198</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>410</v>
+        <v>317</v>
       </c>
       <c r="F99" s="1">
         <v>0</v>
@@ -4147,13 +4156,13 @@
         <v>103</v>
       </c>
       <c r="B100" t="s">
-        <v>411</v>
+        <v>502</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>199</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>412</v>
+        <v>318</v>
       </c>
       <c r="F100" s="1">
         <v>0</v>
@@ -4170,13 +4179,13 @@
         <v>104</v>
       </c>
       <c r="B101" t="s">
-        <v>413</v>
+        <v>503</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>200</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>414</v>
+        <v>319</v>
       </c>
       <c r="F101" s="1">
         <v>0</v>
@@ -4193,13 +4202,13 @@
         <v>105</v>
       </c>
       <c r="B102" t="s">
-        <v>415</v>
+        <v>504</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>201</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>416</v>
+        <v>320</v>
       </c>
       <c r="F102" s="1">
         <v>0</v>
@@ -4211,7 +4220,7 @@
         <v>1</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>417</v>
+        <v>321</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -4219,13 +4228,13 @@
         <v>106</v>
       </c>
       <c r="B103" t="s">
-        <v>418</v>
+        <v>505</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>202</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>419</v>
+        <v>322</v>
       </c>
       <c r="F103" s="1">
         <v>0</v>
@@ -4242,13 +4251,13 @@
         <v>107</v>
       </c>
       <c r="B104" t="s">
-        <v>420</v>
+        <v>506</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>203</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>421</v>
+        <v>323</v>
       </c>
       <c r="F104" s="1">
         <v>0</v>
@@ -4265,13 +4274,13 @@
         <v>108</v>
       </c>
       <c r="B105" t="s">
-        <v>422</v>
+        <v>507</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>204</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>424</v>
+        <v>325</v>
       </c>
       <c r="F105" s="1">
         <v>0</v>
@@ -4288,13 +4297,13 @@
         <v>109</v>
       </c>
       <c r="B106" t="s">
-        <v>425</v>
+        <v>508</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>205</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>426</v>
+        <v>326</v>
       </c>
       <c r="F106" s="1">
         <v>0</v>
@@ -4306,7 +4315,7 @@
         <v>1</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4314,13 +4323,13 @@
         <v>110</v>
       </c>
       <c r="B107" t="s">
-        <v>427</v>
+        <v>509</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>206</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>428</v>
+        <v>327</v>
       </c>
       <c r="F107" s="1">
         <v>0</v>
@@ -4337,13 +4346,13 @@
         <v>111</v>
       </c>
       <c r="B108" t="s">
-        <v>429</v>
+        <v>510</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>207</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>430</v>
+        <v>328</v>
       </c>
       <c r="F108" s="1">
         <v>0</v>
@@ -4360,13 +4369,13 @@
         <v>112</v>
       </c>
       <c r="B109" t="s">
-        <v>431</v>
+        <v>511</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>208</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>434</v>
+        <v>329</v>
       </c>
       <c r="F109" s="1">
         <v>0</v>
@@ -4383,13 +4392,13 @@
         <v>113</v>
       </c>
       <c r="B110" t="s">
-        <v>432</v>
+        <v>512</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>209</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>435</v>
+        <v>330</v>
       </c>
       <c r="F110" s="1">
         <v>0</v>
@@ -4406,13 +4415,13 @@
         <v>114</v>
       </c>
       <c r="B111" t="s">
-        <v>433</v>
+        <v>513</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>210</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>436</v>
+        <v>331</v>
       </c>
       <c r="F111" s="1">
         <v>0</v>
@@ -4429,13 +4438,13 @@
         <v>115</v>
       </c>
       <c r="B112" t="s">
-        <v>438</v>
+        <v>514</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>211</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>439</v>
+        <v>333</v>
       </c>
       <c r="F112" s="1">
         <v>0</v>
@@ -4447,7 +4456,7 @@
         <v>1</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>322</v>
+        <v>271</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -4455,13 +4464,13 @@
         <v>116</v>
       </c>
       <c r="B113" t="s">
-        <v>440</v>
+        <v>515</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>212</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>441</v>
+        <v>334</v>
       </c>
       <c r="F113" s="1">
         <v>0</v>
@@ -4475,84 +4484,84 @@
     </row>
     <row r="114" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>442</v>
+        <v>335</v>
       </c>
       <c r="B114" t="s">
-        <v>496</v>
+        <v>516</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>469</v>
+        <v>362</v>
       </c>
       <c r="F114" s="1">
         <v>1</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>498</v>
+        <v>389</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>443</v>
+        <v>336</v>
       </c>
       <c r="B115" t="s">
-        <v>497</v>
+        <v>517</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>470</v>
+        <v>363</v>
       </c>
       <c r="F115" s="1">
         <v>1</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>498</v>
+        <v>389</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>444</v>
+        <v>337</v>
       </c>
       <c r="B116" t="s">
-        <v>499</v>
+        <v>518</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>471</v>
+        <v>364</v>
       </c>
       <c r="F116" s="1">
         <v>1</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>445</v>
+        <v>338</v>
       </c>
       <c r="B117" t="s">
-        <v>500</v>
+        <v>519</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>472</v>
+        <v>365</v>
       </c>
       <c r="F117" s="1">
         <v>1</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>446</v>
+        <v>339</v>
       </c>
       <c r="B118" t="s">
-        <v>501</v>
+        <v>520</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>473</v>
+        <v>366</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>502</v>
+        <v>390</v>
       </c>
       <c r="F118" s="1">
         <v>0</v>
@@ -4566,16 +4575,16 @@
     </row>
     <row r="119" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>447</v>
+        <v>340</v>
       </c>
       <c r="B119" t="s">
-        <v>503</v>
+        <v>521</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>474</v>
+        <v>367</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>504</v>
+        <v>391</v>
       </c>
       <c r="F119" s="1">
         <v>0</v>
@@ -4589,16 +4598,16 @@
     </row>
     <row r="120" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>448</v>
+        <v>341</v>
       </c>
       <c r="B120" t="s">
-        <v>505</v>
+        <v>522</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>475</v>
+        <v>368</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>475</v>
+        <v>368</v>
       </c>
       <c r="F120" s="1">
         <v>0</v>
@@ -4610,21 +4619,21 @@
         <v>1</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>449</v>
+        <v>342</v>
       </c>
       <c r="B121" t="s">
-        <v>506</v>
+        <v>523</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>476</v>
+        <v>369</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>507</v>
+        <v>392</v>
       </c>
       <c r="F121" s="1">
         <v>0</v>
@@ -4638,16 +4647,16 @@
     </row>
     <row r="122" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>450</v>
+        <v>343</v>
       </c>
       <c r="B122" t="s">
-        <v>508</v>
+        <v>524</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>477</v>
+        <v>370</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>477</v>
+        <v>370</v>
       </c>
       <c r="F122" s="1">
         <v>0</v>
@@ -4659,21 +4668,21 @@
         <v>1</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>451</v>
+        <v>344</v>
       </c>
       <c r="B123" t="s">
-        <v>509</v>
+        <v>525</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>478</v>
+        <v>371</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>510</v>
+        <v>393</v>
       </c>
       <c r="F123" s="1">
         <v>0</v>
@@ -4687,16 +4696,16 @@
     </row>
     <row r="124" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>452</v>
+        <v>345</v>
       </c>
       <c r="B124" t="s">
-        <v>511</v>
+        <v>526</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>479</v>
+        <v>372</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>512</v>
+        <v>394</v>
       </c>
       <c r="F124" s="1">
         <v>0</v>
@@ -4710,36 +4719,36 @@
     </row>
     <row r="125" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>453</v>
+        <v>346</v>
       </c>
       <c r="B125" t="s">
-        <v>513</v>
+        <v>527</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>480</v>
+        <v>373</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>521</v>
+        <v>395</v>
       </c>
       <c r="F125" s="1">
         <v>1</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>454</v>
+        <v>347</v>
       </c>
       <c r="B126" t="s">
-        <v>514</v>
+        <v>528</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>481</v>
+        <v>374</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>522</v>
+        <v>396</v>
       </c>
       <c r="F126" s="1">
         <v>0</v>
@@ -4751,21 +4760,21 @@
         <v>1</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>455</v>
+        <v>348</v>
       </c>
       <c r="B127" t="s">
-        <v>515</v>
+        <v>529</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>482</v>
+        <v>375</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>523</v>
+        <v>397</v>
       </c>
       <c r="F127" s="1">
         <v>0</v>
@@ -4779,16 +4788,16 @@
     </row>
     <row r="128" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>456</v>
+        <v>349</v>
       </c>
       <c r="B128" t="s">
-        <v>516</v>
+        <v>530</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>483</v>
+        <v>376</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>524</v>
+        <v>398</v>
       </c>
       <c r="F128" s="1">
         <v>0</v>
@@ -4802,16 +4811,16 @@
     </row>
     <row r="129" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>457</v>
+        <v>350</v>
       </c>
       <c r="B129" t="s">
-        <v>517</v>
+        <v>531</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>484</v>
+        <v>377</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>525</v>
+        <v>399</v>
       </c>
       <c r="F129" s="1">
         <v>0</v>
@@ -4825,16 +4834,16 @@
     </row>
     <row r="130" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>458</v>
+        <v>351</v>
       </c>
       <c r="B130" t="s">
-        <v>518</v>
+        <v>532</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>485</v>
+        <v>378</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>526</v>
+        <v>400</v>
       </c>
       <c r="F130" s="1">
         <v>0</v>
@@ -4848,16 +4857,16 @@
     </row>
     <row r="131" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>459</v>
+        <v>352</v>
       </c>
       <c r="B131" t="s">
-        <v>519</v>
+        <v>533</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>486</v>
+        <v>379</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>527</v>
+        <v>401</v>
       </c>
       <c r="F131" s="1">
         <v>0</v>
@@ -4871,16 +4880,16 @@
     </row>
     <row r="132" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>460</v>
+        <v>353</v>
       </c>
       <c r="B132" t="s">
-        <v>520</v>
+        <v>534</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>487</v>
+        <v>380</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>528</v>
+        <v>402</v>
       </c>
       <c r="F132" s="1">
         <v>0</v>
@@ -4894,16 +4903,16 @@
     </row>
     <row r="133" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>461</v>
+        <v>354</v>
       </c>
       <c r="B133" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>488</v>
+        <v>381</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>538</v>
+        <v>404</v>
       </c>
       <c r="F133" s="1">
         <v>0</v>
@@ -4915,21 +4924,21 @@
         <v>1</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>539</v>
+        <v>405</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>462</v>
+        <v>355</v>
       </c>
       <c r="B134" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>489</v>
+        <v>382</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>529</v>
+        <v>403</v>
       </c>
       <c r="F134" s="1">
         <v>0</v>
@@ -4943,30 +4952,30 @@
     </row>
     <row r="135" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>463</v>
+        <v>356</v>
       </c>
       <c r="B135" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>490</v>
+        <v>383</v>
       </c>
       <c r="F135" s="1">
         <v>1</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>464</v>
+        <v>357</v>
       </c>
       <c r="B136" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>491</v>
+        <v>384</v>
       </c>
       <c r="F136" s="1">
         <v>1</v>
@@ -4977,13 +4986,13 @@
     </row>
     <row r="137" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>465</v>
+        <v>358</v>
       </c>
       <c r="B137" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>492</v>
+        <v>385</v>
       </c>
       <c r="F137" s="1">
         <v>1</v>
@@ -4994,13 +5003,13 @@
     </row>
     <row r="138" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>466</v>
+        <v>359</v>
       </c>
       <c r="B138" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>493</v>
+        <v>386</v>
       </c>
       <c r="F138" s="1">
         <v>1</v>
@@ -5011,13 +5020,13 @@
     </row>
     <row r="139" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>467</v>
+        <v>360</v>
       </c>
       <c r="B139" t="s">
-        <v>537</v>
+        <v>541</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>494</v>
+        <v>387</v>
       </c>
       <c r="F139" s="1">
         <v>1</v>
@@ -5028,13 +5037,13 @@
     </row>
     <row r="140" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>468</v>
+        <v>361</v>
       </c>
       <c r="B140" t="s">
-        <v>536</v>
+        <v>542</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>495</v>
+        <v>388</v>
       </c>
       <c r="F140" s="1">
         <v>1</v>

</xml_diff>